<commit_message>
Made Ordered even MORE efficient
</commit_message>
<xml_diff>
--- a/experimentalResults/Frequency Distribution Experiental Resultsxlsx.xlsx
+++ b/experimentalResults/Frequency Distribution Experiental Resultsxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bermed28/Desktop/CIIC4020/COURSE RESOURCES/Projects/P2/CIIC4020_Project2/experimentalResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07F661CA-4CCA-5F42-A3B4-DBF2C0E2D4B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F5FF91-7D92-B148-BF6C-6066184C9C65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="2320" windowWidth="28040" windowHeight="17440" xr2:uid="{EB3ADBF1-0B85-A647-B9F0-BE1C7BC0AA5E}"/>
   </bookViews>
@@ -622,64 +622,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>70215.490000000005</c:v>
+                  <c:v>33695.279999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53120.995999999999</c:v>
+                  <c:v>23068.243999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26771.29</c:v>
+                  <c:v>29389.78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47583.34</c:v>
+                  <c:v>33172.695</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57618.11</c:v>
+                  <c:v>30956.425999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74631.58</c:v>
+                  <c:v>30220.115000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>79356.570000000007</c:v>
+                  <c:v>33588.785000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>107833.66</c:v>
+                  <c:v>43545.065999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>113560.82</c:v>
+                  <c:v>40279.163999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>144556.39000000001</c:v>
+                  <c:v>46516.71</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>177486.05</c:v>
+                  <c:v>55686.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>186525.34</c:v>
+                  <c:v>68610.05</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>209918.72</c:v>
+                  <c:v>60287.964999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>242378.2</c:v>
+                  <c:v>63304.714999999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>267284.90000000002</c:v>
+                  <c:v>68542.880000000005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>298387.88</c:v>
+                  <c:v>76550.31</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>331716.53000000003</c:v>
+                  <c:v>82388.149999999994</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>385753.53</c:v>
+                  <c:v>99322.559999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>401947.1</c:v>
+                  <c:v>87800.39</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>448450.4</c:v>
+                  <c:v>94237.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2130,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0AA748-5A07-D74B-8BE7-D14CFA065E6E}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2164,7 +2164,7 @@
         <v>61381.31</v>
       </c>
       <c r="D2">
-        <v>70215.490000000005</v>
+        <v>33695.279999999999</v>
       </c>
       <c r="E2">
         <v>23188.27</v>
@@ -2181,7 +2181,7 @@
         <v>55464.362999999998</v>
       </c>
       <c r="D3">
-        <v>53120.995999999999</v>
+        <v>23068.243999999999</v>
       </c>
       <c r="E3">
         <v>12429.764999999999</v>
@@ -2198,7 +2198,7 @@
         <v>26475.49</v>
       </c>
       <c r="D4">
-        <v>26771.29</v>
+        <v>29389.78</v>
       </c>
       <c r="E4">
         <v>14783.59</v>
@@ -2215,7 +2215,7 @@
         <v>34088.32</v>
       </c>
       <c r="D5">
-        <v>47583.34</v>
+        <v>33172.695</v>
       </c>
       <c r="E5">
         <v>22134.455000000002</v>
@@ -2232,7 +2232,7 @@
         <v>44501.023000000001</v>
       </c>
       <c r="D6">
-        <v>57618.11</v>
+        <v>30956.425999999999</v>
       </c>
       <c r="E6">
         <v>24373.544999999998</v>
@@ -2249,7 +2249,7 @@
         <v>57111.28</v>
       </c>
       <c r="D7">
-        <v>74631.58</v>
+        <v>30220.115000000002</v>
       </c>
       <c r="E7">
         <v>22947.54</v>
@@ -2266,7 +2266,7 @@
         <v>66061.05</v>
       </c>
       <c r="D8">
-        <v>79356.570000000007</v>
+        <v>33588.785000000003</v>
       </c>
       <c r="E8">
         <v>22892.794999999998</v>
@@ -2283,7 +2283,7 @@
         <v>81275.850000000006</v>
       </c>
       <c r="D9">
-        <v>107833.66</v>
+        <v>43545.065999999999</v>
       </c>
       <c r="E9">
         <v>25895.54</v>
@@ -2300,7 +2300,7 @@
         <v>89256.08</v>
       </c>
       <c r="D10">
-        <v>113560.82</v>
+        <v>40279.163999999997</v>
       </c>
       <c r="E10">
         <v>24277.186000000002</v>
@@ -2317,7 +2317,7 @@
         <v>109473.64</v>
       </c>
       <c r="D11">
-        <v>144556.39000000001</v>
+        <v>46516.71</v>
       </c>
       <c r="E11">
         <v>28364.436000000002</v>
@@ -2334,7 +2334,7 @@
         <v>135405.85999999999</v>
       </c>
       <c r="D12">
-        <v>177486.05</v>
+        <v>55686.1</v>
       </c>
       <c r="E12">
         <v>31551.384999999998</v>
@@ -2351,7 +2351,7 @@
         <v>151804.81</v>
       </c>
       <c r="D13">
-        <v>186525.34</v>
+        <v>68610.05</v>
       </c>
       <c r="E13">
         <v>33178.07</v>
@@ -2368,7 +2368,7 @@
         <v>168846.06</v>
       </c>
       <c r="D14">
-        <v>209918.72</v>
+        <v>60287.964999999997</v>
       </c>
       <c r="E14">
         <v>33115.684000000001</v>
@@ -2385,7 +2385,7 @@
         <v>188522.05</v>
       </c>
       <c r="D15">
-        <v>242378.2</v>
+        <v>63304.714999999997</v>
       </c>
       <c r="E15">
         <v>35402.629999999997</v>
@@ -2402,7 +2402,7 @@
         <v>212642.34</v>
       </c>
       <c r="D16">
-        <v>267284.90000000002</v>
+        <v>68542.880000000005</v>
       </c>
       <c r="E16">
         <v>42126.593999999997</v>
@@ -2419,7 +2419,7 @@
         <v>240869.45</v>
       </c>
       <c r="D17">
-        <v>298387.88</v>
+        <v>76550.31</v>
       </c>
       <c r="E17">
         <v>38362.726999999999</v>
@@ -2436,7 +2436,7 @@
         <v>266383.75</v>
       </c>
       <c r="D18">
-        <v>331716.53000000003</v>
+        <v>82388.149999999994</v>
       </c>
       <c r="E18">
         <v>41642.67</v>
@@ -2453,7 +2453,7 @@
         <v>292263.3</v>
       </c>
       <c r="D19">
-        <v>385753.53</v>
+        <v>99322.559999999998</v>
       </c>
       <c r="E19">
         <v>44513.2</v>
@@ -2470,7 +2470,7 @@
         <v>320895.46999999997</v>
       </c>
       <c r="D20">
-        <v>401947.1</v>
+        <v>87800.39</v>
       </c>
       <c r="E20">
         <v>49575.15</v>
@@ -2487,7 +2487,7 @@
         <v>352917.4</v>
       </c>
       <c r="D21">
-        <v>448450.4</v>
+        <v>94237.9</v>
       </c>
       <c r="E21">
         <v>51916.175999999999</v>

</xml_diff>